<commit_message>
arreglando template y deal owner id
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Industrias" sheetId="2" r:id="rId2"/>
     <sheet name="Usuarios" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="DEAL_OWNER">Usuarios!$C$2:$C$30</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
@@ -84,12 +87,6 @@
     <t>appointmentscheduled</t>
   </si>
   <si>
-    <t>Cristian</t>
-  </si>
-  <si>
-    <t>CG</t>
-  </si>
-  <si>
     <t>CATEGORIA DE INDUSTRIA</t>
   </si>
   <si>
@@ -541,13 +538,19 @@
   </si>
   <si>
     <t>email</t>
+  </si>
+  <si>
+    <t>GEN</t>
+  </si>
+  <si>
+    <t>NOTA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,6 +620,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -638,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -649,11 +658,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -929,15 +945,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
@@ -947,13 +963,13 @@
     <col min="8" max="8" width="24.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="29" width="8.7109375" customWidth="1"/>
     <col min="30" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -993,8 +1009,11 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1025,18 +1044,16 @@
       <c r="J2">
         <v>500</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="str">
-        <f>IFERROR(LOOKUP(K2,Usuarios!B:B,Usuarios!A:A),"")</f>
-        <v/>
+      <c r="K2" s="10"/>
+      <c r="L2" t="e">
+        <f>LOOKUP(K2,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1045,9 +1062,13 @@
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
       <c r="I3" s="4"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3" s="10"/>
+      <c r="L3" t="e">
+        <f>LOOKUP(K3,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="E4" s="4"/>
@@ -1055,9 +1076,13 @@
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="10"/>
+      <c r="L4" t="e">
+        <f>LOOKUP(K4,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="C5" s="4"/>
       <c r="E5" s="4"/>
@@ -1065,9 +1090,13 @@
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
       <c r="I5" s="4"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="10"/>
+      <c r="L5" t="e">
+        <f>LOOKUP(K5,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="C6" s="4"/>
       <c r="E6" s="4"/>
@@ -1075,9 +1104,13 @@
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="4"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="10"/>
+      <c r="L6" t="e">
+        <f>LOOKUP(K6,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="C7" s="4"/>
       <c r="E7" s="4"/>
@@ -1085,9 +1118,13 @@
       <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="4"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="10"/>
+      <c r="L7" t="e">
+        <f>LOOKUP(K7,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="C8" s="4"/>
       <c r="E8" s="4"/>
@@ -1095,9 +1132,13 @@
       <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="4"/>
-      <c r="K8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="10"/>
+      <c r="L8" t="e">
+        <f>LOOKUP(K8,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="C9" s="4"/>
       <c r="E9" s="4"/>
@@ -1105,9 +1146,13 @@
       <c r="G9" s="4"/>
       <c r="H9" s="5"/>
       <c r="I9" s="4"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="10"/>
+      <c r="L9" t="e">
+        <f>LOOKUP(K9,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="C10" s="4"/>
       <c r="E10" s="4"/>
@@ -1115,9 +1160,13 @@
       <c r="G10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="4"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="10"/>
+      <c r="L10" t="e">
+        <f>LOOKUP(K10,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="C11" s="4"/>
       <c r="E11" s="4"/>
@@ -1125,9 +1174,13 @@
       <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="4"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="10"/>
+      <c r="L11" t="e">
+        <f>LOOKUP(K11,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="C12" s="4"/>
       <c r="E12" s="4"/>
@@ -1135,9 +1188,13 @@
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
       <c r="I12" s="4"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="10"/>
+      <c r="L12" t="e">
+        <f>LOOKUP(K12,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="C13" s="4"/>
       <c r="E13" s="4"/>
@@ -1145,9 +1202,13 @@
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
       <c r="I13" s="4"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="10"/>
+      <c r="L13" t="e">
+        <f>LOOKUP(K13,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="C14" s="4"/>
       <c r="E14" s="4"/>
@@ -1155,9 +1216,13 @@
       <c r="G14" s="4"/>
       <c r="H14" s="5"/>
       <c r="I14" s="4"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="10"/>
+      <c r="L14" t="e">
+        <f>LOOKUP(K14,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="C15" s="4"/>
       <c r="E15" s="4"/>
@@ -1165,9 +1230,13 @@
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
       <c r="I15" s="4"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="10"/>
+      <c r="L15" t="e">
+        <f>LOOKUP(K15,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="C16" s="4"/>
       <c r="E16" s="4"/>
@@ -1175,9 +1244,13 @@
       <c r="G16" s="4"/>
       <c r="H16" s="5"/>
       <c r="I16" s="4"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="10"/>
+      <c r="L16" t="e">
+        <f>LOOKUP(K16,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="C17" s="4"/>
       <c r="E17" s="4"/>
@@ -1185,9 +1258,13 @@
       <c r="G17" s="4"/>
       <c r="H17" s="5"/>
       <c r="I17" s="4"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="10"/>
+      <c r="L17" t="e">
+        <f>LOOKUP(K17,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="C18" s="4"/>
       <c r="E18" s="4"/>
@@ -1195,9 +1272,13 @@
       <c r="G18" s="4"/>
       <c r="H18" s="5"/>
       <c r="I18" s="4"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="10"/>
+      <c r="L18" t="e">
+        <f>LOOKUP(K18,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="C19" s="4"/>
       <c r="E19" s="4"/>
@@ -1205,9 +1286,13 @@
       <c r="G19" s="4"/>
       <c r="H19" s="5"/>
       <c r="I19" s="4"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="10"/>
+      <c r="L19" t="e">
+        <f>LOOKUP(K19,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="C20" s="4"/>
       <c r="E20" s="4"/>
@@ -1215,9 +1300,13 @@
       <c r="G20" s="4"/>
       <c r="H20" s="5"/>
       <c r="I20" s="4"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="10"/>
+      <c r="L20" t="e">
+        <f>LOOKUP(K20,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" s="4"/>
@@ -1225,9 +1314,13 @@
       <c r="G21" s="4"/>
       <c r="H21" s="5"/>
       <c r="I21" s="4"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="10"/>
+      <c r="L21" t="e">
+        <f>LOOKUP(K21,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="C22" s="4"/>
       <c r="E22" s="4"/>
@@ -1235,36 +1328,68 @@
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
       <c r="I22" s="4"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K27" s="6"/>
-    </row>
-    <row r="28" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K28" s="6"/>
-    </row>
-    <row r="29" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="10"/>
+      <c r="L22" t="e">
+        <f>LOOKUP(K22,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="10"/>
+      <c r="L23" t="e">
+        <f>LOOKUP(K23,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="10"/>
+      <c r="L24" t="e">
+        <f>LOOKUP(K24,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="10"/>
+      <c r="L25" t="e">
+        <f>LOOKUP(K25,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="10"/>
+      <c r="L26" t="e">
+        <f>LOOKUP(K26,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="10"/>
+      <c r="L27" t="e">
+        <f>LOOKUP(K27,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="10"/>
+      <c r="L28" t="e">
+        <f>LOOKUP(K28,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="10"/>
+      <c r="L29" t="e">
+        <f>LOOKUP(K29,Usuarios!B:B,Usuarios!A:A)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K32" s="6"/>
     </row>
     <row r="33" spans="11:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1322,15 +1447,58 @@
       <c r="K50" s="6"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="containsErrors" dxfId="0" priority="1">
+      <formula>ISERROR(L1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="5">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50">
+      <formula1>3</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I45">
+      <formula1>"IGUAL(I2;""apppointmentscheduled"")"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J45">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M45">
+      <formula1>"CG,CM,GEN"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" sqref="L2:L29">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="L2:L29" evalError="1"/>
+  </ignoredErrors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Industrias!$A$2:$A$148</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Usuarios!$B$2:$B$30</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K29</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1338,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A148"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A120" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1350,17 +1518,17 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1370,722 +1538,722 @@
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2098,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2112,16 +2280,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadiendo validacion de datos al excel
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -60,30 +60,12 @@
     <t>PRODUCTO</t>
   </si>
   <si>
-    <t>UNIVERSIDAD DE LOS LLANOS</t>
-  </si>
-  <si>
-    <t>unillanos.edu.co</t>
-  </si>
-  <si>
     <t>Alternative Dispute Resolution</t>
   </si>
   <si>
     <t>CO</t>
   </si>
   <si>
-    <t>Aurelio</t>
-  </si>
-  <si>
-    <t>Cheveroni</t>
-  </si>
-  <si>
-    <t>+358123456</t>
-  </si>
-  <si>
-    <t>aurelio@unillanos.edu.co</t>
-  </si>
-  <si>
     <t>appointmentscheduled</t>
   </si>
   <si>
@@ -544,13 +526,31 @@
   </si>
   <si>
     <t>NOTA</t>
+  </si>
+  <si>
+    <t>EMPRESA DE EJEMPLO</t>
+  </si>
+  <si>
+    <t>ejemplo.com</t>
+  </si>
+  <si>
+    <t>Nombre de contacto</t>
+  </si>
+  <si>
+    <t>Apellido de contacto</t>
+  </si>
+  <si>
+    <t>contacto@ejemplo.com</t>
+  </si>
+  <si>
+    <t>Nota del deal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,6 +626,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -644,10 +652,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,8 +668,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -948,13 +962,13 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="14" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="10" style="1" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
@@ -963,9 +977,10 @@
     <col min="8" max="8" width="24.28515625" customWidth="1"/>
     <col min="9" max="9" width="22.140625" customWidth="1"/>
     <col min="10" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="29" width="8.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="29" width="8.7109375" customWidth="1"/>
     <col min="30" max="1025" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -973,7 +988,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1010,36 +1025,36 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="4">
+        <v>579999999</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="J2">
         <v>500</v>
@@ -1050,12 +1065,15 @@
         <v>#N/A</v>
       </c>
       <c r="M2" t="s">
-        <v>173</v>
+        <v>167</v>
+      </c>
+      <c r="N2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1452,14 +1470,11 @@
       <formula>ISERROR(L1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50">
       <formula1>3</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I45">
-      <formula1>"IGUAL(I2;""apppointmentscheduled"")"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J45">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J46">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M45">
@@ -1467,6 +1482,12 @@
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" sqref="L2:L29">
       <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I50">
+      <formula1>"apppointmentscheduled"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H50">
+      <formula1>LOWER(OR(ISNUMBER(MATCH("*@*.???",A2,0)),ISNUMBER(MATCH("*@*.??",A2,0))))</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1518,742 +1539,742 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="8" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="8" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="8" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="8" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="8" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="8" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="8" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="8" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="8" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2280,16 +2301,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arreglando errores en excel, index y demas
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -962,7 +962,7 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1470,7 @@
       <formula>ISERROR(L1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <dataValidations count="5">
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D50">
       <formula1>3</formula1>
     </dataValidation>
@@ -1485,9 +1485,6 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I50">
       <formula1>"apppointmentscheduled"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H50">
-      <formula1>LOWER(OR(ISNUMBER(MATCH("*@*.???",A2,0)),ISNUMBER(MATCH("*@*.??",A2,0))))</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>